<commit_message>
Commit before fresh test data
</commit_message>
<xml_diff>
--- a/public/Book1.xlsx
+++ b/public/Book1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellurm\Desktop\SAP_File_Executor\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellurm\Desktop\SelfServiceApp\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>E2E_24_PS_ES_RE_Data</t>
   </si>
@@ -32,19 +32,34 @@
     <t>E2E_Intra</t>
   </si>
   <si>
-    <t>E2E_BTS_Bundle</t>
-  </si>
-  <si>
     <t>E2E_CTO_BTS</t>
   </si>
   <si>
     <t>Scenarios</t>
   </si>
+  <si>
+    <t>E2E_BTS_Service</t>
+  </si>
+  <si>
+    <t>E2E_23_RENEWAL_1</t>
+  </si>
+  <si>
+    <t>E2E_23_RENEWAL_2</t>
+  </si>
+  <si>
+    <t>E2E_Installments</t>
+  </si>
+  <si>
+    <t>E2E_20_RFC2</t>
+  </si>
+  <si>
+    <t>E2E_StockRotationReturnDelivery</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,16 +213,17 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="27">
@@ -339,7 +355,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="43"/>
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,28 +477,28 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -526,7 +542,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -539,58 +555,58 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="47">
-    <cellStyle name="20% - Accent1 2" xfId="2"/>
-    <cellStyle name="20% - Accent2 2" xfId="3"/>
-    <cellStyle name="20% - Accent3 2" xfId="4"/>
-    <cellStyle name="20% - Accent4 2" xfId="5"/>
-    <cellStyle name="20% - Accent5 2" xfId="6"/>
-    <cellStyle name="20% - Accent6 2" xfId="7"/>
-    <cellStyle name="40% - Accent1 2" xfId="8"/>
-    <cellStyle name="40% - Accent2 2" xfId="9"/>
-    <cellStyle name="40% - Accent3 2" xfId="10"/>
-    <cellStyle name="40% - Accent4 2" xfId="11"/>
-    <cellStyle name="40% - Accent5 2" xfId="12"/>
-    <cellStyle name="40% - Accent6 2" xfId="13"/>
-    <cellStyle name="60% - Accent1 2" xfId="14"/>
-    <cellStyle name="60% - Accent2 2" xfId="15"/>
-    <cellStyle name="60% - Accent3 2" xfId="16"/>
-    <cellStyle name="60% - Accent4 2" xfId="17"/>
-    <cellStyle name="60% - Accent5 2" xfId="18"/>
-    <cellStyle name="60% - Accent6 2" xfId="19"/>
-    <cellStyle name="Accent1 2" xfId="20"/>
-    <cellStyle name="Accent2 2" xfId="21"/>
-    <cellStyle name="Accent3 2" xfId="22"/>
-    <cellStyle name="Accent4 2" xfId="23"/>
-    <cellStyle name="Accent5 2" xfId="24"/>
-    <cellStyle name="Accent6 2" xfId="25"/>
-    <cellStyle name="Bad 2" xfId="27"/>
-    <cellStyle name="Bad 3" xfId="26"/>
-    <cellStyle name="Calculation 2" xfId="28"/>
-    <cellStyle name="Check Cell 2" xfId="29"/>
-    <cellStyle name="Explanatory Text 2" xfId="30"/>
-    <cellStyle name="Good 2" xfId="32"/>
-    <cellStyle name="Good 3" xfId="31"/>
-    <cellStyle name="Heading 1 2" xfId="33"/>
-    <cellStyle name="Heading 2 2" xfId="34"/>
-    <cellStyle name="Heading 3 2" xfId="35"/>
-    <cellStyle name="Heading 4 2" xfId="36"/>
-    <cellStyle name="Hyperlink 2" xfId="37"/>
-    <cellStyle name="Input 2" xfId="38"/>
-    <cellStyle name="Linked Cell 2" xfId="39"/>
-    <cellStyle name="Neutral 2" xfId="40"/>
+    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Bad 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Bad 3" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Calculation 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Check Cell 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Good 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Good 3" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Heading 1 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Heading 2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Heading 3 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Heading 4 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Input 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Neutral 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="41"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Note 2" xfId="42"/>
-    <cellStyle name="Output 2" xfId="43"/>
-    <cellStyle name="Title 2" xfId="44"/>
-    <cellStyle name="Total 2" xfId="45"/>
-    <cellStyle name="Warning Text 2" xfId="46"/>
+    <cellStyle name="Normal 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Note 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Output 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Title 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Total 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Warning Text 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -867,41 +883,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated unstable to failure
</commit_message>
<xml_diff>
--- a/public/Book1.xlsx
+++ b/public/Book1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>E2E_24_PS_ES_RE_Data</t>
   </si>
   <si>
-    <t>E2E_Intra</t>
-  </si>
-  <si>
     <t>E2E_CTO_BTS</t>
   </si>
   <si>
@@ -53,7 +50,13 @@
     <t>E2E_20_RFC2</t>
   </si>
   <si>
-    <t>E2E_StockRotationReturnDelivery</t>
+    <t>E2E_BTS_Bundle</t>
+  </si>
+  <si>
+    <t>E2E_StockRotationReturn</t>
+  </si>
+  <si>
+    <t>E2E_LocalCurr</t>
   </si>
 </sst>
 </file>
@@ -884,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +900,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -907,17 +910,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -936,13 +939,18 @@
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>